<commit_message>
Commiting - second commit
</commit_message>
<xml_diff>
--- a/API data.xlsx
+++ b/API data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>firstname</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>dinner</t>
+  </si>
+  <si>
+    <t>Akhila</t>
+  </si>
+  <si>
+    <t>Batchu</t>
+  </si>
+  <si>
+    <t>lunch</t>
   </si>
 </sst>
 </file>
@@ -367,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -425,6 +434,29 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>345</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44682</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45078</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>